<commit_message>
新增每周Presentation, Gantt Chart week5, Back ground settings
</commit_message>
<xml_diff>
--- a/DesignDocuments/SFX/Sound Assets Request.xlsx
+++ b/DesignDocuments/SFX/Sound Assets Request.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC125D2-04C9-4F44-82A4-B4B5926D55FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mechanics" sheetId="2" r:id="rId1"/>
@@ -16,12 +17,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>作者</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -32,7 +33,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="140">
   <si>
     <t>Combat</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -600,23 +601,32 @@
   <si>
     <t>Only exists on enemies' body. The weak point has the same function as a jump point. When weak point beaten, enemies suffer more damage from any kind of attack （floating &amp; rotating knife damage not included). Now, the weak point represented by shinning rune or enemies's head.</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StepingOn_RockWood</t>
+  </si>
+  <si>
+    <t>木头地面踩踏</t>
+  </si>
+  <si>
+    <t>Cloth shoes steping on wood road.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -766,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -807,6 +817,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -821,7 +834,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -837,7 +850,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -912,6 +925,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -947,6 +977,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1122,14 +1169,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="3"/>
     <col min="2" max="2" width="17.6640625" style="1" customWidth="1"/>
@@ -1137,7 +1184,7 @@
     <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="20.399999999999999">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
@@ -1148,7 +1195,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="42" customHeight="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1159,7 +1206,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="42" customHeight="1">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1170,7 +1217,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="42" customHeight="1">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1181,7 +1228,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="42" customHeight="1">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1192,7 +1239,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="42" customHeight="1">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1203,7 +1250,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="78" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="78">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1214,7 +1261,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="31.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1225,486 +1272,486 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3">
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3">
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3">
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3">
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3">
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3">
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3">
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3">
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3">
       <c r="B41" s="7"/>
       <c r="C41" s="8"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3">
       <c r="B42" s="7"/>
       <c r="C42" s="8"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3">
       <c r="B43" s="7"/>
       <c r="C43" s="8"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3">
       <c r="B44" s="7"/>
       <c r="C44" s="8"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3">
       <c r="B45" s="7"/>
       <c r="C45" s="8"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3">
       <c r="B46" s="7"/>
       <c r="C46" s="8"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3">
       <c r="B47" s="7"/>
       <c r="C47" s="8"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3">
       <c r="B48" s="7"/>
       <c r="C48" s="8"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3">
       <c r="B49" s="7"/>
       <c r="C49" s="8"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3">
       <c r="B50" s="7"/>
       <c r="C50" s="8"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3">
       <c r="B51" s="7"/>
       <c r="C51" s="8"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3">
       <c r="B52" s="7"/>
       <c r="C52" s="8"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3">
       <c r="B53" s="7"/>
       <c r="C53" s="8"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3">
       <c r="B54" s="7"/>
       <c r="C54" s="8"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3">
       <c r="B55" s="7"/>
       <c r="C55" s="8"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3">
       <c r="B56" s="7"/>
       <c r="C56" s="8"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3">
       <c r="B57" s="7"/>
       <c r="C57" s="8"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3">
       <c r="B58" s="7"/>
       <c r="C58" s="8"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3">
       <c r="B59" s="7"/>
       <c r="C59" s="8"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3">
       <c r="B60" s="7"/>
       <c r="C60" s="8"/>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3">
       <c r="B61" s="7"/>
       <c r="C61" s="8"/>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3">
       <c r="B62" s="7"/>
       <c r="C62" s="8"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3">
       <c r="B63" s="7"/>
       <c r="C63" s="8"/>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3">
       <c r="B64" s="7"/>
       <c r="C64" s="8"/>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3">
       <c r="B65" s="7"/>
       <c r="C65" s="8"/>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3">
       <c r="B66" s="7"/>
       <c r="C66" s="8"/>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3">
       <c r="B67" s="7"/>
       <c r="C67" s="8"/>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3">
       <c r="B68" s="7"/>
       <c r="C68" s="8"/>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3">
       <c r="B69" s="7"/>
       <c r="C69" s="8"/>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3">
       <c r="B70" s="7"/>
       <c r="C70" s="8"/>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3">
       <c r="B71" s="7"/>
       <c r="C71" s="8"/>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:3">
       <c r="B72" s="7"/>
       <c r="C72" s="8"/>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3">
       <c r="B73" s="7"/>
       <c r="C73" s="8"/>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3">
       <c r="B74" s="7"/>
       <c r="C74" s="8"/>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:3">
       <c r="B75" s="7"/>
       <c r="C75" s="8"/>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:3">
       <c r="B76" s="7"/>
       <c r="C76" s="8"/>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:3">
       <c r="B77" s="7"/>
       <c r="C77" s="8"/>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:3">
       <c r="B78" s="7"/>
       <c r="C78" s="8"/>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:3">
       <c r="B79" s="7"/>
       <c r="C79" s="8"/>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:3">
       <c r="B80" s="7"/>
       <c r="C80" s="8"/>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:3">
       <c r="B81" s="7"/>
       <c r="C81" s="8"/>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:3">
       <c r="B82" s="7"/>
       <c r="C82" s="8"/>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:3">
       <c r="B83" s="7"/>
       <c r="C83" s="8"/>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:3">
       <c r="B84" s="7"/>
       <c r="C84" s="8"/>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:3">
       <c r="B85" s="7"/>
       <c r="C85" s="8"/>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:3">
       <c r="B86" s="7"/>
       <c r="C86" s="8"/>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:3">
       <c r="B87" s="7"/>
       <c r="C87" s="8"/>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:3">
       <c r="B88" s="7"/>
       <c r="C88" s="8"/>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:3">
       <c r="B89" s="7"/>
       <c r="C89" s="8"/>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:3">
       <c r="B90" s="7"/>
       <c r="C90" s="8"/>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:3">
       <c r="B91" s="7"/>
       <c r="C91" s="8"/>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:3">
       <c r="B92" s="7"/>
       <c r="C92" s="8"/>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:3">
       <c r="B93" s="7"/>
       <c r="C93" s="8"/>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:3">
       <c r="B94" s="7"/>
       <c r="C94" s="8"/>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:3">
       <c r="B95" s="7"/>
       <c r="C95" s="8"/>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:3">
       <c r="B96" s="7"/>
       <c r="C96" s="8"/>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:3">
       <c r="B97" s="7"/>
       <c r="C97" s="8"/>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:3">
       <c r="B98" s="7"/>
       <c r="C98" s="8"/>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:3">
       <c r="B99" s="7"/>
       <c r="C99" s="8"/>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:3">
       <c r="B100" s="7"/>
       <c r="C100" s="8"/>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:3">
       <c r="B101" s="7"/>
       <c r="C101" s="8"/>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:3">
       <c r="B102" s="7"/>
       <c r="C102" s="8"/>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:3">
       <c r="B103" s="7"/>
       <c r="C103" s="8"/>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:3">
       <c r="B104" s="7"/>
       <c r="C104" s="8"/>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:3">
       <c r="B105" s="7"/>
       <c r="C105" s="8"/>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:3">
       <c r="B106" s="7"/>
       <c r="C106" s="8"/>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:3">
       <c r="B107" s="7"/>
       <c r="C107" s="8"/>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:3">
       <c r="B108" s="7"/>
       <c r="C108" s="8"/>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:3">
       <c r="B109" s="7"/>
       <c r="C109" s="8"/>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:3">
       <c r="B110" s="7"/>
       <c r="C110" s="8"/>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:3">
       <c r="B111" s="7"/>
       <c r="C111" s="8"/>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:3">
       <c r="B112" s="7"/>
       <c r="C112" s="8"/>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:3">
       <c r="B113" s="7"/>
       <c r="C113" s="8"/>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:3">
       <c r="B114" s="7"/>
       <c r="C114" s="8"/>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3">
       <c r="B115" s="7"/>
       <c r="C115" s="8"/>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3">
       <c r="B116" s="7"/>
       <c r="C116" s="8"/>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:3">
       <c r="B117" s="7"/>
       <c r="C117" s="8"/>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:3">
       <c r="B118" s="7"/>
       <c r="C118" s="8"/>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3">
       <c r="B119" s="7"/>
       <c r="C119" s="8"/>
     </row>
@@ -1716,17 +1763,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="2" customWidth="1"/>
     <col min="2" max="3" width="5.88671875" style="1" customWidth="1"/>
@@ -1738,41 +1785,41 @@
     <col min="11" max="16384" width="8.88671875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="16" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:10" s="16" customFormat="1" ht="16.2" customHeight="1">
+      <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="19" t="s">
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="18"/>
+    <row r="2" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A2" s="19"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="3">
         <v>1</v>
       </c>
@@ -1782,13 +1829,13 @@
       <c r="I2" s="3">
         <v>3</v>
       </c>
-      <c r="J2" s="19"/>
-    </row>
-    <row r="3" spans="1:10" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="J2" s="20"/>
+    </row>
+    <row r="3" spans="1:10" ht="31.2">
+      <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="3"/>
@@ -1806,9 +1853,9 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="20"/>
+    <row r="4" spans="1:10" ht="31.2">
+      <c r="A4" s="22"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
         <v>48</v>
@@ -1824,9 +1871,9 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="20"/>
+    <row r="5" spans="1:10" ht="31.2">
+      <c r="A5" s="22"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="3">
         <v>5</v>
       </c>
@@ -1844,9 +1891,9 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="20"/>
+    <row r="6" spans="1:10" ht="31.2">
+      <c r="A6" s="22"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="3">
         <v>5</v>
       </c>
@@ -1864,9 +1911,9 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="20"/>
+    <row r="7" spans="1:10" ht="31.2">
+      <c r="A7" s="22"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="3">
         <v>5</v>
       </c>
@@ -1884,9 +1931,9 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="20"/>
+    <row r="8" spans="1:10" ht="31.2">
+      <c r="A8" s="22"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="3">
         <v>5</v>
       </c>
@@ -1904,9 +1951,9 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="20"/>
+    <row r="9" spans="1:10" ht="15.6">
+      <c r="A9" s="22"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="3">
         <v>4</v>
       </c>
@@ -1924,9 +1971,9 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="20"/>
+    <row r="10" spans="1:10" ht="31.2">
+      <c r="A10" s="22"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="3">
         <v>4</v>
       </c>
@@ -1944,9 +1991,9 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="20"/>
+    <row r="11" spans="1:10" ht="31.2">
+      <c r="A11" s="22"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="3">
         <v>3</v>
       </c>
@@ -1964,9 +2011,9 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="46.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="20"/>
+    <row r="12" spans="1:10" ht="46.8">
+      <c r="A12" s="22"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="3">
         <v>3</v>
       </c>
@@ -1984,9 +2031,9 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="20"/>
+    <row r="13" spans="1:10" ht="15.6">
+      <c r="A13" s="22"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="3">
         <v>5</v>
       </c>
@@ -2004,9 +2051,9 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="20"/>
+    <row r="14" spans="1:10" ht="15.6">
+      <c r="A14" s="22"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -2016,9 +2063,9 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="20"/>
+    <row r="15" spans="1:10" ht="15.6">
+      <c r="A15" s="22"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -2028,9 +2075,9 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:10" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="20" t="s">
+    <row r="16" spans="1:10" ht="31.2">
+      <c r="A16" s="22"/>
+      <c r="B16" s="21" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="3">
@@ -2050,9 +2097,9 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="20"/>
+    <row r="17" spans="1:10" ht="31.2">
+      <c r="A17" s="22"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="3">
         <v>4</v>
       </c>
@@ -2070,9 +2117,9 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="20"/>
+    <row r="18" spans="1:10" ht="31.2">
+      <c r="A18" s="22"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="3">
         <v>4</v>
       </c>
@@ -2090,9 +2137,9 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="20"/>
+    <row r="19" spans="1:10" ht="15.6">
+      <c r="A19" s="22"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="3">
         <v>3</v>
       </c>
@@ -2110,9 +2157,9 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="20"/>
+    <row r="20" spans="1:10" ht="31.2">
+      <c r="A20" s="22"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="3">
         <v>3</v>
       </c>
@@ -2130,9 +2177,9 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="20"/>
+    <row r="21" spans="1:10" ht="31.2">
+      <c r="A21" s="22"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="3">
         <v>2</v>
       </c>
@@ -2150,9 +2197,9 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="20"/>
+    <row r="22" spans="1:10" ht="46.8">
+      <c r="A22" s="22"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="3">
         <v>3</v>
       </c>
@@ -2170,9 +2217,9 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="20"/>
+    <row r="23" spans="1:10" ht="15.6">
+      <c r="A23" s="22"/>
+      <c r="B23" s="21"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -2182,9 +2229,9 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="20" t="s">
+    <row r="24" spans="1:10" ht="15.6" customHeight="1">
+      <c r="A24" s="22"/>
+      <c r="B24" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="3"/>
@@ -2196,9 +2243,9 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="20"/>
+    <row r="25" spans="1:10" ht="15.6">
+      <c r="A25" s="22"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -2208,9 +2255,9 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="20"/>
+    <row r="26" spans="1:10" ht="15.6">
+      <c r="A26" s="22"/>
+      <c r="B26" s="21"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -2220,9 +2267,9 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" s="20"/>
+    <row r="27" spans="1:10" ht="15.6">
+      <c r="A27" s="22"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -2232,9 +2279,9 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="20"/>
+    <row r="28" spans="1:10" ht="15.6">
+      <c r="A28" s="22"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -2244,9 +2291,9 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="20"/>
+    <row r="29" spans="1:10" ht="15.6">
+      <c r="A29" s="22"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -2256,9 +2303,9 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
-      <c r="B30" s="20" t="s">
+    <row r="30" spans="1:10" ht="15.6">
+      <c r="A30" s="22"/>
+      <c r="B30" s="21" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="3">
@@ -2278,9 +2325,9 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
-      <c r="B31" s="20"/>
+    <row r="31" spans="1:10" ht="15.6">
+      <c r="A31" s="22"/>
+      <c r="B31" s="21"/>
       <c r="C31" s="3">
         <v>2</v>
       </c>
@@ -2298,9 +2345,9 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
-      <c r="B32" s="20"/>
+    <row r="32" spans="1:10" ht="15.6">
+      <c r="A32" s="22"/>
+      <c r="B32" s="21"/>
       <c r="C32" s="3">
         <v>2</v>
       </c>
@@ -2318,9 +2365,9 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
-      <c r="B33" s="20"/>
+    <row r="33" spans="1:10" ht="15.6">
+      <c r="A33" s="22"/>
+      <c r="B33" s="21"/>
       <c r="C33" s="3">
         <v>2</v>
       </c>
@@ -2338,9 +2385,9 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
-      <c r="B34" s="20"/>
+    <row r="34" spans="1:10" ht="15.6">
+      <c r="A34" s="22"/>
+      <c r="B34" s="21"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -2350,9 +2397,9 @@
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="20"/>
+    <row r="35" spans="1:10" ht="15.6">
+      <c r="A35" s="22"/>
+      <c r="B35" s="21"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -2362,9 +2409,9 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
-      <c r="B36" s="20"/>
+    <row r="36" spans="1:10" ht="15.6">
+      <c r="A36" s="22"/>
+      <c r="B36" s="21"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -2374,8 +2421,8 @@
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
+    <row r="37" spans="1:10" ht="15.6">
+      <c r="A37" s="22"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -2386,8 +2433,8 @@
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
+    <row r="38" spans="1:10" ht="15.6">
+      <c r="A38" s="22"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -2398,8 +2445,8 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
+    <row r="39" spans="1:10" ht="15.6">
+      <c r="A39" s="22"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -2410,8 +2457,8 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
+    <row r="40" spans="1:10" ht="15.6">
+      <c r="A40" s="22"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -2422,8 +2469,8 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
+    <row r="41" spans="1:10" ht="15.6">
+      <c r="A41" s="22"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -2434,8 +2481,8 @@
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="21" t="s">
+    <row r="42" spans="1:10" ht="30.6" customHeight="1">
+      <c r="A42" s="22" t="s">
         <v>117</v>
       </c>
       <c r="B42" s="3"/>
@@ -2456,8 +2503,8 @@
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
     </row>
-    <row r="43" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
+    <row r="43" spans="1:10" ht="30.6" customHeight="1">
+      <c r="A43" s="22"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3">
         <v>5</v>
@@ -2476,142 +2523,150 @@
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3">
+    <row r="44" spans="1:10" ht="30.6" customHeight="1">
+      <c r="A44" s="22"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18">
         <v>5</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>31</v>
+      <c r="D44" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>138</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-    </row>
-    <row r="45" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="21"/>
+        <v>139</v>
+      </c>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+    </row>
+    <row r="45" spans="1:10" ht="30.6" customHeight="1">
+      <c r="A45" s="22"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3">
         <v>5</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
+    <row r="46" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A46" s="22"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
     </row>
-    <row r="47" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="21"/>
+    <row r="47" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A47" s="22"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3">
         <v>4</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
     </row>
-    <row r="48" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="21"/>
+    <row r="48" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A48" s="22"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
     </row>
-    <row r="49" spans="1:10" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="21"/>
+    <row r="49" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A49" s="22"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>118</v>
+        <v>20</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>121</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
     </row>
-    <row r="50" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="21"/>
+    <row r="50" spans="1:10" ht="34.799999999999997" customHeight="1">
+      <c r="A50" s="22"/>
       <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="3"/>
+      <c r="C50" s="3">
+        <v>3</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
     </row>
-    <row r="51" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="21"/>
+    <row r="51" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A51" s="22"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -2622,82 +2677,82 @@
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
     </row>
-    <row r="52" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="18" t="s">
-        <v>24</v>
-      </c>
+    <row r="52" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A52" s="22"/>
       <c r="B52" s="3"/>
-      <c r="C52" s="3">
-        <v>3</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>109</v>
-      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="8"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
     </row>
-    <row r="53" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
+    <row r="53" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A53" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3">
         <v>3</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
     </row>
-    <row r="54" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="18"/>
+    <row r="54" spans="1:10" ht="31.2" customHeight="1">
+      <c r="A54" s="19"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3">
         <v>3</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
     </row>
-    <row r="55" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="18"/>
+    <row r="55" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A55" s="19"/>
       <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="8"/>
+      <c r="C55" s="3">
+        <v>3</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>111</v>
+      </c>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
     </row>
-    <row r="56" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="18"/>
+    <row r="56" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A56" s="19"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -2708,8 +2763,8 @@
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
     </row>
-    <row r="57" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="18"/>
+    <row r="57" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A57" s="19"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -2720,8 +2775,8 @@
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
     </row>
-    <row r="58" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="18"/>
+    <row r="58" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A58" s="19"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -2732,8 +2787,8 @@
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
     </row>
-    <row r="59" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="18"/>
+    <row r="59" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A59" s="19"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -2744,8 +2799,8 @@
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
     </row>
-    <row r="60" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="18"/>
+    <row r="60" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A60" s="19"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -2756,8 +2811,8 @@
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
     </row>
-    <row r="61" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="18"/>
+    <row r="61" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A61" s="19"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -2768,10 +2823,8 @@
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
     </row>
-    <row r="62" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
-        <v>47</v>
-      </c>
+    <row r="62" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A62" s="19"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -2782,8 +2835,10 @@
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
     </row>
-    <row r="63" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="18"/>
+    <row r="63" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A63" s="19" t="s">
+        <v>47</v>
+      </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -2794,8 +2849,8 @@
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
     </row>
-    <row r="64" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="18"/>
+    <row r="64" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A64" s="19"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -2806,8 +2861,8 @@
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
     </row>
-    <row r="65" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="18"/>
+    <row r="65" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A65" s="19"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -2818,8 +2873,8 @@
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
     </row>
-    <row r="66" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="18"/>
+    <row r="66" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A66" s="19"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -2830,8 +2885,8 @@
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
     </row>
-    <row r="67" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="18"/>
+    <row r="67" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A67" s="19"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -2842,8 +2897,8 @@
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
     </row>
-    <row r="68" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="18"/>
+    <row r="68" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A68" s="19"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -2854,8 +2909,8 @@
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
     </row>
-    <row r="69" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="18"/>
+    <row r="69" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A69" s="19"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -2866,8 +2921,8 @@
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
     </row>
-    <row r="70" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="18"/>
+    <row r="70" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A70" s="19"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -2878,8 +2933,8 @@
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
     </row>
-    <row r="71" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="18"/>
+    <row r="71" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A71" s="19"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
@@ -2890,8 +2945,8 @@
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
     </row>
-    <row r="72" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="18"/>
+    <row r="72" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A72" s="19"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
@@ -2902,8 +2957,8 @@
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
     </row>
-    <row r="73" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="18"/>
+    <row r="73" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A73" s="19"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
@@ -2914,15 +2969,27 @@
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
     </row>
+    <row r="74" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A74" s="19"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="8"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="A52:A61"/>
+    <mergeCell ref="A63:A74"/>
+    <mergeCell ref="A53:A62"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="B3:B15"/>
     <mergeCell ref="B24:B29"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A42:A51"/>
+    <mergeCell ref="A42:A52"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="E1:E2"/>
@@ -2934,7 +3001,19 @@
     <mergeCell ref="B30:B36"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C3:C73">
+  <conditionalFormatting sqref="C3:C43 C45:C74">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2952,11 +3031,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>'Hiding Data'!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>J3:J313</xm:sqref>
+          <xm:sqref>J3:J314</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2965,35 +3044,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="23" style="10" customWidth="1"/>
     <col min="2" max="16384" width="8.88671875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="12" customFormat="1" ht="16.8" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" s="12" customFormat="1" ht="16.8" thickBot="1">
       <c r="A1" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1">
       <c r="A3" s="13" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1">
       <c r="A4" s="14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1">
       <c r="A5" s="15" t="s">
         <v>133</v>
       </c>

</xml_diff>